<commit_message>
Add symbol "minus" to table
</commit_message>
<xml_diff>
--- a/7seg.xlsx
+++ b/7seg.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>8B</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>1,3,5,6,7</t>
+  </si>
+  <si>
+    <t>"-"</t>
   </si>
 </sst>
 </file>
@@ -446,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:U30"/>
+  <dimension ref="A3:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+      <selection activeCell="V31" sqref="V31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -698,7 +701,7 @@
         <v>0</v>
       </c>
       <c r="T7" s="1" t="str">
-        <f t="shared" ref="T7:T30" si="0">"0x"&amp;DEC2HEX(D7*1+E7*2+F7*4+G7*8+H7*16+I7*32+J7*64+K7*128+L7*256+M7*512+N7*1024+O7*2048+P7*4096+Q7*8192+R7*16384+S7*32768)</f>
+        <f t="shared" ref="T7:T32" si="0">"0x"&amp;DEC2HEX(D7*1+E7*2+F7*4+G7*8+H7*16+I7*32+J7*64+K7*128+L7*256+M7*512+N7*1024+O7*2048+P7*4096+Q7*8192+R7*16384+S7*32768)</f>
         <v>0x840</v>
       </c>
     </row>
@@ -1243,731 +1246,851 @@
       </c>
     </row>
     <row r="17" spans="1:20">
-      <c r="B17" s="2"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
+      <c r="B17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1</v>
+      </c>
+      <c r="M17" s="1">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1">
+        <v>0</v>
+      </c>
+      <c r="P17" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>0</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0</v>
+      </c>
+      <c r="T17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>0x100</v>
+      </c>
     </row>
     <row r="18" spans="1:20">
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" s="1">
+      <c r="B18" s="2"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
         <v>2</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G19" s="1">
         <v>3</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H19" s="1">
         <v>4</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I19" s="1">
         <v>5</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J19" s="1">
         <v>6</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K19" s="1">
         <v>7</v>
       </c>
-      <c r="L18" s="1">
+      <c r="L19" s="1">
         <v>8</v>
       </c>
-      <c r="M18" s="1">
+      <c r="M19" s="1">
         <v>9</v>
       </c>
-      <c r="N18" s="1">
+      <c r="N19" s="1">
         <v>10</v>
       </c>
-      <c r="O18" s="1">
+      <c r="O19" s="1">
         <v>11</v>
       </c>
-      <c r="P18" s="1">
+      <c r="P19" s="1">
         <v>12</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="Q19" s="1">
         <v>13</v>
       </c>
-      <c r="R18" s="1">
+      <c r="R19" s="1">
         <v>14</v>
       </c>
-      <c r="S18" s="1">
+      <c r="S19" s="1">
         <v>15</v>
       </c>
-      <c r="T18" s="1"/>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="D19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="T19" s="1"/>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="D20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="O20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="P20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="Q20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R19" s="1" t="s">
+      <c r="R20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S19" s="1" t="s">
+      <c r="S20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T19" s="1"/>
-    </row>
-    <row r="20" spans="1:20">
       <c r="T20" s="1"/>
     </row>
     <row r="21" spans="1:20">
-      <c r="A21" t="s">
+      <c r="T21" s="1"/>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="1">
-        <v>0</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
-      <c r="F21" s="1">
-        <v>1</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1</v>
-      </c>
-      <c r="H21" s="1">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1">
-        <v>0</v>
-      </c>
-      <c r="J21" s="1">
-        <v>0</v>
-      </c>
-      <c r="K21" s="1">
-        <v>0</v>
-      </c>
-      <c r="L21" s="1">
-        <v>0</v>
-      </c>
-      <c r="M21" s="1">
-        <v>0</v>
-      </c>
-      <c r="N21" s="1">
-        <v>0</v>
-      </c>
-      <c r="O21" s="1">
-        <v>0</v>
-      </c>
-      <c r="P21" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>1</v>
-      </c>
-      <c r="R21" s="1">
-        <v>1</v>
-      </c>
-      <c r="S21" s="1">
-        <v>0</v>
-      </c>
-      <c r="T21" s="1" t="str">
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <v>0</v>
+      </c>
+      <c r="P22" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>1</v>
+      </c>
+      <c r="R22" s="1">
+        <v>1</v>
+      </c>
+      <c r="S22" s="1">
+        <v>0</v>
+      </c>
+      <c r="T22" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0x700E</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
+    <row r="23" spans="1:20">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="1">
-        <v>0</v>
-      </c>
-      <c r="E22" s="1">
-        <v>1</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0</v>
-      </c>
-      <c r="G22" s="1">
-        <v>0</v>
-      </c>
-      <c r="H22" s="1">
-        <v>0</v>
-      </c>
-      <c r="I22" s="1">
-        <v>0</v>
-      </c>
-      <c r="J22" s="1">
-        <v>0</v>
-      </c>
-      <c r="K22" s="1">
-        <v>0</v>
-      </c>
-      <c r="L22" s="1">
-        <v>0</v>
-      </c>
-      <c r="M22" s="1">
-        <v>0</v>
-      </c>
-      <c r="N22" s="1">
-        <v>0</v>
-      </c>
-      <c r="O22" s="1">
-        <v>0</v>
-      </c>
-      <c r="P22" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="1">
-        <v>0</v>
-      </c>
-      <c r="R22" s="1">
-        <v>0</v>
-      </c>
-      <c r="S22" s="1">
-        <v>0</v>
-      </c>
-      <c r="T22" s="1" t="str">
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
+      <c r="O23" s="1">
+        <v>0</v>
+      </c>
+      <c r="P23" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>0</v>
+      </c>
+      <c r="R23" s="1">
+        <v>0</v>
+      </c>
+      <c r="S23" s="1">
+        <v>0</v>
+      </c>
+      <c r="T23" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0x1002</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
-      <c r="B23">
+    <row r="24" spans="1:20">
+      <c r="B24">
         <v>2</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="1">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0</v>
-      </c>
-      <c r="F23" s="1">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1">
-        <v>1</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0</v>
-      </c>
-      <c r="I23" s="1">
-        <v>0</v>
-      </c>
-      <c r="J23" s="1">
-        <v>0</v>
-      </c>
-      <c r="K23" s="1">
-        <v>0</v>
-      </c>
-      <c r="L23" s="1">
-        <v>0</v>
-      </c>
-      <c r="M23" s="1">
-        <v>0</v>
-      </c>
-      <c r="N23" s="1">
-        <v>0</v>
-      </c>
-      <c r="O23" s="1">
-        <v>0</v>
-      </c>
-      <c r="P23" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="1">
-        <v>0</v>
-      </c>
-      <c r="R23" s="1">
-        <v>1</v>
-      </c>
-      <c r="S23" s="1">
-        <v>1</v>
-      </c>
-      <c r="T23" s="1" t="str">
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1">
+        <v>0</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0</v>
+      </c>
+      <c r="O24" s="1">
+        <v>0</v>
+      </c>
+      <c r="P24" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>0</v>
+      </c>
+      <c r="R24" s="1">
+        <v>1</v>
+      </c>
+      <c r="S24" s="1">
+        <v>1</v>
+      </c>
+      <c r="T24" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0xD00C</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
-      <c r="B24">
+    <row r="25" spans="1:20">
+      <c r="B25">
         <v>3</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-      <c r="E24" s="1">
-        <v>1</v>
-      </c>
-      <c r="F24" s="1">
-        <v>0</v>
-      </c>
-      <c r="G24" s="1">
-        <v>1</v>
-      </c>
-      <c r="H24" s="1">
-        <v>0</v>
-      </c>
-      <c r="I24" s="1">
-        <v>0</v>
-      </c>
-      <c r="J24" s="1">
-        <v>0</v>
-      </c>
-      <c r="K24" s="1">
-        <v>0</v>
-      </c>
-      <c r="L24" s="1">
-        <v>0</v>
-      </c>
-      <c r="M24" s="1">
-        <v>0</v>
-      </c>
-      <c r="N24" s="1">
-        <v>0</v>
-      </c>
-      <c r="O24" s="1">
-        <v>0</v>
-      </c>
-      <c r="P24" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q24" s="1">
-        <v>0</v>
-      </c>
-      <c r="R24" s="1">
-        <v>1</v>
-      </c>
-      <c r="S24" s="1">
-        <v>1</v>
-      </c>
-      <c r="T24" s="1" t="str">
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0</v>
+      </c>
+      <c r="O25" s="1">
+        <v>0</v>
+      </c>
+      <c r="P25" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>0</v>
+      </c>
+      <c r="R25" s="1">
+        <v>1</v>
+      </c>
+      <c r="S25" s="1">
+        <v>1</v>
+      </c>
+      <c r="T25" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0xD00A</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
-      <c r="B25">
+    <row r="26" spans="1:20">
+      <c r="B26">
         <v>4</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="1">
-        <v>0</v>
-      </c>
-      <c r="E25" s="1">
-        <v>1</v>
-      </c>
-      <c r="F25" s="1">
-        <v>0</v>
-      </c>
-      <c r="G25" s="1">
-        <v>0</v>
-      </c>
-      <c r="H25" s="1">
-        <v>0</v>
-      </c>
-      <c r="I25" s="1">
-        <v>0</v>
-      </c>
-      <c r="J25" s="1">
-        <v>0</v>
-      </c>
-      <c r="K25" s="1">
-        <v>0</v>
-      </c>
-      <c r="L25" s="1">
-        <v>0</v>
-      </c>
-      <c r="M25" s="1">
-        <v>0</v>
-      </c>
-      <c r="N25" s="1">
-        <v>0</v>
-      </c>
-      <c r="O25" s="1">
-        <v>0</v>
-      </c>
-      <c r="P25" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="1">
-        <v>1</v>
-      </c>
-      <c r="R25" s="1">
-        <v>0</v>
-      </c>
-      <c r="S25" s="1">
-        <v>1</v>
-      </c>
-      <c r="T25" s="1" t="str">
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0</v>
+      </c>
+      <c r="O26" s="1">
+        <v>0</v>
+      </c>
+      <c r="P26" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>1</v>
+      </c>
+      <c r="R26" s="1">
+        <v>0</v>
+      </c>
+      <c r="S26" s="1">
+        <v>1</v>
+      </c>
+      <c r="T26" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0xB002</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
-      <c r="B26">
+    <row r="27" spans="1:20">
+      <c r="B27">
         <v>5</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="1">
-        <v>0</v>
-      </c>
-      <c r="E26" s="1">
-        <v>1</v>
-      </c>
-      <c r="F26" s="1">
-        <v>0</v>
-      </c>
-      <c r="G26" s="1">
-        <v>1</v>
-      </c>
-      <c r="H26" s="1">
-        <v>0</v>
-      </c>
-      <c r="I26" s="1">
-        <v>0</v>
-      </c>
-      <c r="J26" s="1">
-        <v>0</v>
-      </c>
-      <c r="K26" s="1">
-        <v>0</v>
-      </c>
-      <c r="L26" s="1">
-        <v>0</v>
-      </c>
-      <c r="M26" s="1">
-        <v>0</v>
-      </c>
-      <c r="N26" s="1">
-        <v>0</v>
-      </c>
-      <c r="O26" s="1">
-        <v>0</v>
-      </c>
-      <c r="P26" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="1">
-        <v>1</v>
-      </c>
-      <c r="R26" s="1">
-        <v>1</v>
-      </c>
-      <c r="S26" s="1">
-        <v>1</v>
-      </c>
-      <c r="T26" s="1" t="str">
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1">
+        <v>0</v>
+      </c>
+      <c r="M27" s="1">
+        <v>0</v>
+      </c>
+      <c r="N27" s="1">
+        <v>0</v>
+      </c>
+      <c r="O27" s="1">
+        <v>0</v>
+      </c>
+      <c r="P27" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>1</v>
+      </c>
+      <c r="R27" s="1">
+        <v>1</v>
+      </c>
+      <c r="S27" s="1">
+        <v>1</v>
+      </c>
+      <c r="T27" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0xE00A</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
-      <c r="B27">
+    <row r="28" spans="1:20">
+      <c r="B28">
         <v>6</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="1">
-        <v>0</v>
-      </c>
-      <c r="E27" s="1">
-        <v>1</v>
-      </c>
-      <c r="F27" s="1">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1">
-        <v>1</v>
-      </c>
-      <c r="H27" s="1">
-        <v>0</v>
-      </c>
-      <c r="I27" s="1">
-        <v>0</v>
-      </c>
-      <c r="J27" s="1">
-        <v>0</v>
-      </c>
-      <c r="K27" s="1">
-        <v>0</v>
-      </c>
-      <c r="L27" s="1">
-        <v>0</v>
-      </c>
-      <c r="M27" s="1">
-        <v>0</v>
-      </c>
-      <c r="N27" s="1">
-        <v>0</v>
-      </c>
-      <c r="O27" s="1">
-        <v>0</v>
-      </c>
-      <c r="P27" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="1">
-        <v>1</v>
-      </c>
-      <c r="R27" s="1">
-        <v>1</v>
-      </c>
-      <c r="S27" s="1">
-        <v>1</v>
-      </c>
-      <c r="T27" s="1" t="str">
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+      <c r="L28" s="1">
+        <v>0</v>
+      </c>
+      <c r="M28" s="1">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1">
+        <v>0</v>
+      </c>
+      <c r="O28" s="1">
+        <v>0</v>
+      </c>
+      <c r="P28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>1</v>
+      </c>
+      <c r="R28" s="1">
+        <v>1</v>
+      </c>
+      <c r="S28" s="1">
+        <v>1</v>
+      </c>
+      <c r="T28" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0xE00E</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
-      <c r="B28">
+    <row r="29" spans="1:20">
+      <c r="B29">
         <v>7</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="1">
-        <v>0</v>
-      </c>
-      <c r="E28" s="1">
-        <v>1</v>
-      </c>
-      <c r="F28" s="1">
-        <v>0</v>
-      </c>
-      <c r="G28" s="1">
-        <v>0</v>
-      </c>
-      <c r="H28" s="1">
-        <v>0</v>
-      </c>
-      <c r="I28" s="1">
-        <v>0</v>
-      </c>
-      <c r="J28" s="1">
-        <v>0</v>
-      </c>
-      <c r="K28" s="1">
-        <v>0</v>
-      </c>
-      <c r="L28" s="1">
-        <v>0</v>
-      </c>
-      <c r="M28" s="1">
-        <v>0</v>
-      </c>
-      <c r="N28" s="1">
-        <v>0</v>
-      </c>
-      <c r="O28" s="1">
-        <v>0</v>
-      </c>
-      <c r="P28" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q28" s="1">
-        <v>0</v>
-      </c>
-      <c r="R28" s="1">
-        <v>1</v>
-      </c>
-      <c r="S28" s="1">
-        <v>0</v>
-      </c>
-      <c r="T28" s="1" t="str">
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+      <c r="L29" s="1">
+        <v>0</v>
+      </c>
+      <c r="M29" s="1">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1">
+        <v>0</v>
+      </c>
+      <c r="O29" s="1">
+        <v>0</v>
+      </c>
+      <c r="P29" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>0</v>
+      </c>
+      <c r="R29" s="1">
+        <v>1</v>
+      </c>
+      <c r="S29" s="1">
+        <v>0</v>
+      </c>
+      <c r="T29" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0x5002</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
-      <c r="B29">
+    <row r="30" spans="1:20">
+      <c r="B30">
         <v>8</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="1">
-        <v>0</v>
-      </c>
-      <c r="E29" s="1">
-        <v>1</v>
-      </c>
-      <c r="F29" s="1">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1">
-        <v>1</v>
-      </c>
-      <c r="H29" s="1">
-        <v>0</v>
-      </c>
-      <c r="I29" s="1">
-        <v>0</v>
-      </c>
-      <c r="J29" s="1">
-        <v>0</v>
-      </c>
-      <c r="K29" s="1">
-        <v>0</v>
-      </c>
-      <c r="L29" s="1">
-        <v>0</v>
-      </c>
-      <c r="M29" s="1">
-        <v>0</v>
-      </c>
-      <c r="N29" s="1">
-        <v>0</v>
-      </c>
-      <c r="O29" s="1">
-        <v>0</v>
-      </c>
-      <c r="P29" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q29" s="1">
-        <v>1</v>
-      </c>
-      <c r="R29" s="1">
-        <v>1</v>
-      </c>
-      <c r="S29" s="1">
-        <v>1</v>
-      </c>
-      <c r="T29" s="1" t="str">
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+      <c r="L30" s="1">
+        <v>0</v>
+      </c>
+      <c r="M30" s="1">
+        <v>0</v>
+      </c>
+      <c r="N30" s="1">
+        <v>0</v>
+      </c>
+      <c r="O30" s="1">
+        <v>0</v>
+      </c>
+      <c r="P30" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>1</v>
+      </c>
+      <c r="R30" s="1">
+        <v>1</v>
+      </c>
+      <c r="S30" s="1">
+        <v>1</v>
+      </c>
+      <c r="T30" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0xF00E</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
-      <c r="B30">
+    <row r="31" spans="1:20">
+      <c r="B31">
         <v>9</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="1">
-        <v>0</v>
-      </c>
-      <c r="E30" s="1">
-        <v>1</v>
-      </c>
-      <c r="F30" s="1">
-        <v>0</v>
-      </c>
-      <c r="G30" s="1">
-        <v>1</v>
-      </c>
-      <c r="H30" s="1">
-        <v>0</v>
-      </c>
-      <c r="I30" s="1">
-        <v>0</v>
-      </c>
-      <c r="J30" s="1">
-        <v>0</v>
-      </c>
-      <c r="K30" s="1">
-        <v>0</v>
-      </c>
-      <c r="L30" s="1">
-        <v>0</v>
-      </c>
-      <c r="M30" s="1">
-        <v>0</v>
-      </c>
-      <c r="N30" s="1">
-        <v>0</v>
-      </c>
-      <c r="O30" s="1">
-        <v>0</v>
-      </c>
-      <c r="P30" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q30" s="1">
-        <v>1</v>
-      </c>
-      <c r="R30" s="1">
-        <v>1</v>
-      </c>
-      <c r="S30" s="1">
-        <v>1</v>
-      </c>
-      <c r="T30" s="1" t="str">
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0</v>
+      </c>
+      <c r="L31" s="1">
+        <v>0</v>
+      </c>
+      <c r="M31" s="1">
+        <v>0</v>
+      </c>
+      <c r="N31" s="1">
+        <v>0</v>
+      </c>
+      <c r="O31" s="1">
+        <v>0</v>
+      </c>
+      <c r="P31" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>1</v>
+      </c>
+      <c r="R31" s="1">
+        <v>1</v>
+      </c>
+      <c r="S31" s="1">
+        <v>1</v>
+      </c>
+      <c r="T31" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0xF00A</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1">
+        <v>0</v>
+      </c>
+      <c r="M32" s="1">
+        <v>0</v>
+      </c>
+      <c r="N32" s="1">
+        <v>0</v>
+      </c>
+      <c r="O32" s="1">
+        <v>0</v>
+      </c>
+      <c r="P32" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>0</v>
+      </c>
+      <c r="R32" s="1">
+        <v>0</v>
+      </c>
+      <c r="S32" s="1">
+        <v>1</v>
+      </c>
+      <c r="T32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>0x8000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>